<commit_message>
updates to plotting funcs and archiving of data csvs
</commit_message>
<xml_diff>
--- a/BISC_OUT/Spectra_Metadata.xlsx
+++ b/BISC_OUT/Spectra_Metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Algae</t>
   </si>
   <si>
-    <t xml:space="preserve">cells/mL</t>
+    <t xml:space="preserve">cells/mL(measured)</t>
   </si>
   <si>
     <t xml:space="preserve">g/ice</t>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t xml:space="preserve">cells/mL_rom_ppb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2DBA_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cells/mL2DBA</t>
   </si>
   <si>
     <t xml:space="preserve">22_7_SB2</t>
@@ -280,8 +286,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.00E+00"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -353,11 +359,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,21 +380,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34:M34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.68"/>
@@ -398,6 +404,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,19 +451,25 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1101</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -482,19 +499,25 @@
         <f aca="false">H2/(0.94)*(1/0.917)/10</f>
         <v>11601.1972435555</v>
       </c>
+      <c r="N2" s="0" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>6174</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1111</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2</v>
@@ -524,19 +547,26 @@
         <f aca="false">H3/(0.94)*(1/0.917)/10</f>
         <v>8700.89793266665</v>
       </c>
+      <c r="N3" s="0" t="n">
+        <v>0.997728028739568</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <f aca="false">1E-034*N3*EXP(87.015*N3)</f>
+        <v>5049.96556216556</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1121</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -566,20 +596,26 @@
         <f aca="false">H4/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="0" t="n">
+        <v>0.999216423664904</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <f aca="false">1E-034*N4*EXP(87.015*N4)</f>
+        <v>5756.81736343492</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1157</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>400</v>
@@ -606,22 +642,28 @@
         <f aca="false">H5/(0.94)*(1/0.917)/10</f>
         <v>5800.59862177777</v>
       </c>
+      <c r="N5" s="0" t="n">
+        <v>1.0003</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>6333</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1037</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>500</v>
@@ -645,22 +687,29 @@
         <f aca="false">H6/(0.94)*(1/0.917)/10</f>
         <v>5800.59862177777</v>
       </c>
+      <c r="N6" s="0" t="n">
+        <v>0.99927795185688</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <f aca="false">1E-034*N6*EXP(87.015*N6)</f>
+        <v>5788.07768897922</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1055</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>750</v>
@@ -684,22 +733,29 @@
         <f aca="false">H7/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N7" s="0" t="n">
+        <v>0.999262334554645</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <f aca="false">1E-034*N7*EXP(87.015*N7)</f>
+        <v>5780.12704668693</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1152</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>400</v>
@@ -726,19 +782,26 @@
         <f aca="false">H8/(0.94)*(1/0.917)/10</f>
         <v>8700.89793266665</v>
       </c>
+      <c r="N8" s="0" t="n">
+        <v>0.998803629079593</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <f aca="false">1E-034*N8*EXP(87.015*N8)</f>
+        <v>5551.4117036814</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1302</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>2</v>
@@ -768,22 +831,29 @@
         <f aca="false">H9/(0.94)*(1/0.917)/10</f>
         <v>17401.7958653333</v>
       </c>
+      <c r="N9" s="0" t="n">
+        <v>1.00112869911369</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <f aca="false">1E-034*N9*EXP(87.015*N9)</f>
+        <v>6812.05185593202</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1134</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>450</v>
@@ -807,19 +877,26 @@
         <f aca="false">H10/(0.94)*(1/0.917)/10</f>
         <v>11601.1972435555</v>
       </c>
+      <c r="N10" s="0" t="n">
+        <v>0.999930747488734</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <f aca="false">1E-034*N10*EXP(87.015*N10)</f>
+        <v>6130.37729530327</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1333</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>500</v>
@@ -846,22 +923,29 @@
         <f aca="false">H11/(0.94)*(1/0.917)/10</f>
         <v>8700.89793266665</v>
       </c>
+      <c r="N11" s="0" t="n">
+        <v>0.999337107150623</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <f aca="false">1E-034*N11*EXP(87.015*N11)</f>
+        <v>5818.29245027628</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1117</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>550</v>
@@ -888,19 +972,26 @@
         <f aca="false">H12/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N12" s="0" t="n">
+        <v>0.999667713536561</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <f aca="false">1E-034*N12*EXP(87.015*N12)</f>
+        <v>5990.08325435433</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1244</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>850</v>
@@ -927,19 +1018,26 @@
         <f aca="false">H13/(0.94)*(1/0.917)/10</f>
         <v>23202.3944871111</v>
       </c>
+      <c r="N13" s="0" t="n">
+        <v>0.999394804902704</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <f aca="false">1E-034*N13*EXP(87.015*N13)</f>
+        <v>5847.91466122582</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>1305</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>3</v>
@@ -969,19 +1067,26 @@
         <f aca="false">H14/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N14" s="0" t="n">
+        <v>0.998352729027748</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">1E-034*N14*EXP(87.015*N14)</f>
+        <v>5335.40953886087</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>1230</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
@@ -1011,19 +1116,26 @@
         <f aca="false">H15/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N15" s="0" t="n">
+        <v>1.00096376999254</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">1E-034*N15*EXP(87.015*N15)</f>
+        <v>6713.8819180794</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>1132</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>400</v>
@@ -1050,19 +1162,26 @@
         <f aca="false">H16/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N16" s="0" t="n">
+        <v>0.998899201733255</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <f aca="false">1E-034*N16*EXP(87.015*N16)</f>
+        <v>5598.30679199597</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1143</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
@@ -1089,19 +1208,26 @@
         <f aca="false">H17/(0.94)*(1/0.917)/10</f>
         <v>8700.89793266665</v>
       </c>
+      <c r="N17" s="0" t="n">
+        <v>0.999400676271843</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <f aca="false">1E-034*N17*EXP(87.015*N17)</f>
+        <v>5850.93748131194</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>1235</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
@@ -1128,22 +1254,29 @@
         <f aca="false">H18/(0.94)*(1/0.917)/10</f>
         <v>17401.7958653333</v>
       </c>
+      <c r="N18" s="0" t="n">
+        <v>0.997791919799729</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <f aca="false">1E-034*N18*EXP(87.015*N18)</f>
+        <v>5078.44411950204</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>1055</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>750</v>
@@ -1167,19 +1300,26 @@
         <f aca="false">H19/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N19" s="0" t="n">
+        <v>0.999262334554645</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <f aca="false">1E-034*N19*EXP(87.015*N19)</f>
+        <v>5780.12704668693</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>1108</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>10</v>
@@ -1206,22 +1346,29 @@
         <f aca="false">H20/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N20" s="0" t="n">
+        <v>1.00180364473015</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <f aca="false">1E-034*N20*EXP(87.015*N20)</f>
+        <v>7228.97839625261</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1007</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>59</v>
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>450</v>
@@ -1245,19 +1392,26 @@
         <f aca="false">H21/(0.94)*(1/0.917)/10</f>
         <v>11601.1972435555</v>
       </c>
+      <c r="N21" s="0" t="n">
+        <v>1.00005768918511</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <f aca="false">1E-034*N21*EXP(87.015*N21)</f>
+        <v>6199.25467542321</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>1220</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>5</v>
@@ -1284,19 +1438,26 @@
         <f aca="false">H22/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N22" s="0" t="n">
+        <v>0.999456975476871</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <f aca="false">1E-034*N22*EXP(87.015*N22)</f>
+        <v>5880.00203692252</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>1233</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>5</v>
@@ -1326,19 +1487,26 @@
         <f aca="false">H23/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N23" s="0" t="n">
+        <v>1.00180364473015</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <f aca="false">1E-034*N23*EXP(87.015*N23)</f>
+        <v>7228.97839625261</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>1247</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>2</v>
@@ -1368,19 +1536,26 @@
         <f aca="false">H24/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N24" s="0" t="n">
+        <v>0.999596077624139</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <f aca="false">1E-034*N24*EXP(87.015*N24)</f>
+        <v>5952.434227211</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>1200</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>2</v>
@@ -1407,19 +1582,26 @@
         <f aca="false">H25/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N25" s="0" t="n">
+        <v>0.999743346860701</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <f aca="false">1E-034*N25*EXP(87.015*N25)</f>
+        <v>6030.09159328888</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>1358</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>3</v>
@@ -1449,19 +1631,26 @@
         <f aca="false">H26/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N26" s="0" t="n">
+        <v>0.997493061731166</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <f aca="false">1E-034*N26*EXP(87.015*N26)</f>
+        <v>4946.5988522209</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>1104</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>900</v>
@@ -1485,19 +1674,26 @@
         <f aca="false">H27/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N27" s="0" t="n">
+        <v>0.998090066749557</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <f aca="false">1E-034*N27*EXP(87.015*N27)</f>
+        <v>5213.47676184949</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>1046</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>400</v>
@@ -1521,19 +1717,26 @@
         <f aca="false">H28/(0.94)*(1/0.917)/10</f>
         <v>14501.4965544444</v>
       </c>
+      <c r="N28" s="0" t="n">
+        <v>0.998859719334347</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <f aca="false">1E-034*N28*EXP(87.015*N28)</f>
+        <v>5578.88594941689</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>1310</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>400</v>
@@ -1557,19 +1760,26 @@
         <f aca="false">H29/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N29" s="0" t="n">
+        <v>0.999171594116956</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <f aca="false">1E-034*N29*EXP(87.015*N29)</f>
+        <v>5734.14739233022</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>1209</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>3</v>
@@ -1599,19 +1809,26 @@
         <f aca="false">H30/(0.94)*(1/0.917)/10</f>
         <v>29002.9931088888</v>
       </c>
+      <c r="N30" s="0" t="n">
+        <v>0.997172132666332</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <f aca="false">1E-034*N30*EXP(87.015*N30)</f>
+        <v>4808.82518439545</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>1159</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2</v>
@@ -1641,19 +1858,26 @@
         <f aca="false">H31/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N31" s="0" t="n">
+        <v>0.997820679177718</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <f aca="false">1E-034*N31*EXP(87.015*N31)</f>
+        <v>5091.31557007718</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>1200</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>400</v>
@@ -1680,19 +1904,26 @@
         <f aca="false">H32/(0.94)*(1/0.917)/10</f>
         <v>23202.3944871111</v>
       </c>
+      <c r="N32" s="0" t="n">
+        <v>0.998519805358618</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <f aca="false">1E-034*N32*EXP(87.015*N32)</f>
+        <v>5414.4490563052</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>1142</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>700</v>
@@ -1719,6 +1950,18 @@
         <f aca="false">H33/(0.94)*(1/0.917)/10</f>
         <v>2320.23944871111</v>
       </c>
+      <c r="N33" s="0" t="n">
+        <v>0.999178426545775</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <f aca="false">1E-034*N33*EXP(87.015*N33)</f>
+        <v>5737.59672693862</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="N34" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>